<commit_message>
Corrections in calculations were made. Important update: a dict introduced in antennas.py that will determine which antenna to use in each frequency range.
</commit_message>
<xml_diff>
--- a/antenna_factors/AH010.xlsx
+++ b/antenna_factors/AH010.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drobjev\PycharmProjects\CISPR 25 Test Site Validation Calcs\antenna_factors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omega\PycharmProjects\CISPR25 Test Site Validation Calcs\antenna_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -9097,7 +9097,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>